<commit_message>
updated ExperStrat-WSX, Platform filters test cases
</commit_message>
<xml_diff>
--- a/InputFiles/TC12_CDS_Filter_ExprStrtgies-WXS.xlsx
+++ b/InputFiles/TC12_CDS_Filter_ExprStrtgies-WXS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epishinavv\git\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593E44CB-E862-4207-A2C5-4C2DE2A4CD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21177326-23EC-426A-B260-1CE548887ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -67,6 +67,19 @@
 OPTIONAL MATCH (p)&lt;--(samp:sample)
 MATCH (samp)&lt;--(f:file)
 WHERE f.experimental_strategy_and_data_subtypes in ['WXS']
+OPTIONAL MATCH (p)&lt;--(diag:diagnosis)
+WITH DISTINCT samp,diag,s,p,f
+RETURN
+    count(distinct s) AS Studies,
+    count(distinct p) AS Participants,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Files`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(p:participant)
+OPTIONAL MATCH (p)&lt;--(samp:sample)
+MATCH (samp)&lt;--(f:file)
+WHERE f.experimental_strategy_and_data_subtypes in ['WXS']
 WITH p, s, collect(distinct samp.sample_id) as samp
 RETURN   
  coalesce(p.participant_id,'') as `Participant ID`,
@@ -75,21 +88,6 @@
  coalesce(p.gender,'') as `Gender`,
  coalesce(apoc.text.join(samp, ','), '') as `Samples`
 ORDER By p.participant_id LIMIT 100</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)
-OPTIONAL MATCH (s)&lt;--(f:file)
-WITH
-    s,f,
-    apoc.text.split(f.experimental_strategy_and_data_subtypes,"[;,]\\s{0,1}") AS experimental_strategies
-WHERE "WXS" in experimental_strategies
-OPTIONAL MATCH (s)&lt;--(p:participant)&lt;--(samp:sample)
-WITH DISTINCT s,f,p,samp
-RETURN
-    count(distinct s) AS Studies,
-    count(distinct p) AS Participants,
-    count(distinct samp) AS Samples,
-    count(distinct f) AS `Files`</t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;--(p:participant)&lt;--(samp:sample)
@@ -499,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,15 +526,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="217" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="186" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -545,7 +543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="217" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="186" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -553,7 +551,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -562,7 +560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="217" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="186" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -570,7 +568,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>

</xml_diff>